<commit_message>
R is not right is think
</commit_message>
<xml_diff>
--- a/exp5/exp5.xlsx
+++ b/exp5/exp5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="8" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t xml:space="preserve">L = </t>
   </si>
@@ -106,12 +106,15 @@
   <si>
     <t>delta C</t>
   </si>
+  <si>
+    <t>I Think we need to change B3 to 219.5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +131,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -153,11 +163,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1717,7 +1728,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -7105,8 +7115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7114,6 +7124,7 @@
     <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -7235,6 +7246,9 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F11" s="1"/>
+    </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
@@ -7251,6 +7265,11 @@
       <c r="B13" s="1">
         <f>B9/B12</f>
         <v>2195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="83" customHeight="1" x14ac:dyDescent="1">
+      <c r="A15" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -7283,6 +7302,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7816,7 +7836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixing excel, adding last exp graph, continuing further with report
</commit_message>
<xml_diff>
--- a/exp5/exp5.xlsx
+++ b/exp5/exp5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6948" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="8" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t xml:space="preserve">L = </t>
   </si>
@@ -109,6 +109,9 @@
   <si>
     <t>I Think we need to change B3 to 219.5</t>
   </si>
+  <si>
+    <t>f0</t>
+  </si>
 </sst>
 </file>
 
@@ -163,12 +166,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2755,6 +2759,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>V vs. f</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2793,6 +2822,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>V0c+V0l</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -2927,6 +2959,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>V0c</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -3055,6 +3090,73 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-B459-4147-853E-A486DDDBD4C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>f0</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'7'!$E$2:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5340</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5340</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'7'!$F$2:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E085-4779-9FBD-E1B4803382B3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3090,6 +3192,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>f [Hz]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3135,6 +3292,7 @@
         <c:axId val="385203984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="6"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3152,6 +3310,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>V</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> [V]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3201,6 +3419,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -6159,15 +6408,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>38517</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>99392</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>269597</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>178906</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6513,18 +6762,18 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.15625" customWidth="1"/>
+    <col min="3" max="3" width="12.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.3671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6546,7 +6795,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6561,7 +6810,7 @@
         <v>9.9999999999999995E-8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -6575,23 +6824,23 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="5">
         <f>1/(SQRT(B2*B1)*2*PI())</f>
         <v>5032.9212104487033</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="5">
         <f>SQRT(1/(2*PI()))*SQRT((D1/(2*(SQRT(B1*B2))))^2+(D2*SQRT(B1)/(2*B2^1.5))^2)</f>
         <v>1.4104739588693904</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -6606,16 +6855,16 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <f>ABS(B5-B4)/(D4^2+D5^2)</f>
-        <v>1.1676389002836397E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <f>ABS(B5-B4)/SQRT(D4^2+D5^2)</f>
+        <v>2.3353358734398135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -6623,7 +6872,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -6634,7 +6883,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -6645,54 +6894,67 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <f>B9/B3</f>
-        <v>4.5019157088122604E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <f>B10/B3</f>
+        <v>1.4846743295019157E-2</v>
+      </c>
+      <c r="C12">
+        <f>SQRT((C10/B3)^2+(B10*D3/B3^2)^2)</f>
+        <v>4.9959483834585034E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="5">
         <f>B9/B12</f>
-        <v>104.4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+        <v>316.56774193548387</v>
+      </c>
+      <c r="C13">
+        <f>SQRT((C9/B12)^2+(B9*C12/B12^2)^2)</f>
+        <v>1.1172216134454935</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="5">
         <f>(1/B13)*SQRT(B1/B2)</f>
-        <v>0.3029001590199597</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+        <v>9.9892605634242029E-2</v>
+      </c>
+      <c r="C19">
+        <f>SQRT((SQRT(B1/B2)*C13/B13^2)^2+(D1/(2*B13*SQRT(B1*B2)))^2+(SQRT(B1)*D2/(2*B13*SQRT(B2^3)))^2)</f>
+        <v>1.1173895531089434E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="1">
         <f>B5/B19</f>
-        <v>18157.798324686835</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+        <v>55059.13040388911</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="1">
         <f>B5-B20/2</f>
-        <v>-3578.8991623434176</v>
+        <v>-22029.565201944555</v>
       </c>
       <c r="C22" s="1">
         <f>B5+B20/2</f>
-        <v>14578.899162343418</v>
+        <v>33029.565201944555</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6700,13 +6962,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="C14" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
@@ -6720,7 +6982,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3">
         <v>1000</v>
       </c>
@@ -6735,7 +6997,7 @@
         <v>0.55581395348837215</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3">
         <v>2000</v>
       </c>
@@ -6750,7 +7012,7 @@
         <v>0.75128205128205139</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
         <v>3000</v>
       </c>
@@ -6765,7 +7027,7 @@
         <v>0.81052631578947376</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
         <v>4000</v>
       </c>
@@ -6780,7 +7042,7 @@
         <v>0.84324324324324318</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3">
         <v>5000</v>
       </c>
@@ -6795,7 +7057,7 @@
         <v>0.86027397260273974</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3">
         <v>6000</v>
       </c>
@@ -6810,7 +7072,7 @@
         <v>0.86027397260273974</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3">
         <v>7000</v>
       </c>
@@ -6825,7 +7087,7 @@
         <v>0.84864864864864864</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3">
         <v>8000</v>
       </c>
@@ -6840,7 +7102,7 @@
         <v>0.84594594594594585</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3">
         <v>9000</v>
       </c>
@@ -6855,7 +7117,7 @@
         <v>0.82666666666666666</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3">
         <v>10000</v>
       </c>
@@ -6870,7 +7132,7 @@
         <v>0.81052631578947376</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3">
         <v>11000</v>
       </c>
@@ -6885,7 +7147,7 @@
         <v>0.8052631578947369</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3">
         <v>12000</v>
       </c>
@@ -6900,7 +7162,7 @@
         <v>0.78441558441558445</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3">
         <v>13000</v>
       </c>
@@ -6915,7 +7177,7 @@
         <v>0.76666666666666672</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3">
         <v>14000</v>
       </c>
@@ -6930,7 +7192,7 @@
         <v>0.7564102564102565</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3">
         <v>15000</v>
       </c>
@@ -6945,7 +7207,7 @@
         <v>0.74615384615384617</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3">
         <v>16000</v>
       </c>
@@ -6960,7 +7222,7 @@
         <v>0.72658227848101264</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3">
         <v>17000</v>
       </c>
@@ -6975,7 +7237,7 @@
         <v>0.71250000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3">
         <v>20000</v>
       </c>
@@ -6990,7 +7252,7 @@
         <v>0.65609756097560978</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3">
         <v>25000</v>
       </c>
@@ -7005,7 +7267,7 @@
         <v>0.58837209302325577</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3">
         <v>30000</v>
       </c>
@@ -7020,7 +7282,7 @@
         <v>0.52045454545454539</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3">
         <v>35000</v>
       </c>
@@ -7035,7 +7297,7 @@
         <v>0.46304347826086956</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3">
         <v>40000</v>
       </c>
@@ -7050,7 +7312,7 @@
         <v>0.41914893617021276</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3">
         <v>500</v>
       </c>
@@ -7065,7 +7327,7 @@
         <v>0.33473684210526317</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3">
         <v>1500</v>
       </c>
@@ -7080,28 +7342,28 @@
         <v>0.67560975609756102</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D33" s="2"/>
     </row>
   </sheetData>
@@ -7115,19 +7377,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.41796875" customWidth="1"/>
+    <col min="3" max="3" width="12.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.3671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7148,7 +7410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -7163,7 +7425,7 @@
         <v>1E-8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -7177,23 +7439,23 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="5">
         <f>1/(SQRT(B2*B1)*2*PI())</f>
         <v>5032.9212104487033</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="5">
         <f>SQRT(1/(2*PI()))*SQRT((D1/(2*(SQRT(B1*B2))))^2+(D2*SQRT(B1)/(2*B2^1.5))^2)</f>
         <v>14.104739588693906</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -7204,19 +7466,19 @@
         <v>6</v>
       </c>
       <c r="D5" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
-        <f>ABS(B5-B4)/(D4^2+D5^2)</f>
-        <v>0.11377739815617381</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="1">
+        <f>ABS(B5-B4)/SQRT(D4^2+D5^2)</f>
+        <v>2.0382009345739767</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -7224,7 +7486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -7235,7 +7497,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -7246,58 +7508,70 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <f>B9/B3</f>
-        <v>1.9225512528473803E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <f>B10/B3</f>
+        <v>1.4669703872437358E-2</v>
+      </c>
+      <c r="C12">
+        <f>SQRT((C10/B3)^2+(B10*D3/B3^2)^2)</f>
+        <v>3.3493731707487145E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1">
         <f>B9/B12</f>
-        <v>219.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="83" customHeight="1" x14ac:dyDescent="1">
+        <v>287.66770186335401</v>
+      </c>
+      <c r="C13">
+        <f>SQRT((C9/B12)^2+(B9*C12/B12^2)^2)</f>
+        <v>6.576840020220529</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="83.05" customHeight="1" x14ac:dyDescent="1.65">
       <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="1">
         <f>(1/B13)*SQRT(B1/B2)</f>
-        <v>1.4406731936985784</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1.099281441637304</v>
+      </c>
+      <c r="C19">
+        <f>SQRT((SQRT(B1/B2)*C13/B13^2)^2+(D1/(2*B13*SQRT(B1*B2)))^2+(SQRT(B1)*D2/(2*B13*SQRT(B2^3)))^2)</f>
+        <v>0.12544674905681827</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="1">
         <f>B5/B19</f>
-        <v>3706.6005138131623</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4857.7186858048271</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="1">
         <f>B5-B20/2</f>
-        <v>3486.6997430934189</v>
+        <v>2911.1406570975864</v>
       </c>
       <c r="C22" s="1">
         <f>B5+B20/2</f>
-        <v>7193.3002569065811</v>
+        <v>7768.8593429024131</v>
       </c>
     </row>
   </sheetData>
@@ -7314,9 +7588,9 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -7330,7 +7604,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>3000</v>
       </c>
@@ -7345,7 +7619,7 @@
         <v>0.47708333333333336</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>3500</v>
       </c>
@@ -7360,7 +7634,7 @@
         <v>0.55744680851063833</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>4000</v>
       </c>
@@ -7375,7 +7649,7 @@
         <v>0.63695652173913053</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>4500</v>
       </c>
@@ -7390,7 +7664,7 @@
         <v>0.71011235955056184</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>5000</v>
       </c>
@@ -7405,7 +7679,7 @@
         <v>0.74545454545454537</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>5100</v>
       </c>
@@ -7420,7 +7694,7 @@
         <v>0.74999999999999989</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>5200</v>
       </c>
@@ -7435,7 +7709,7 @@
         <v>0.74999999999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>5300</v>
       </c>
@@ -7450,7 +7724,7 @@
         <v>0.74999999999999989</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>5400</v>
       </c>
@@ -7465,7 +7739,7 @@
         <v>0.74999999999999989</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>5500</v>
       </c>
@@ -7480,7 +7754,7 @@
         <v>0.74999999999999989</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>5600</v>
       </c>
@@ -7495,7 +7769,7 @@
         <v>0.74999999999999989</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>5700</v>
       </c>
@@ -7510,7 +7784,7 @@
         <v>0.74545454545454537</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>5800</v>
       </c>
@@ -7525,7 +7799,7 @@
         <v>0.74545454545454537</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>5900</v>
       </c>
@@ -7540,7 +7814,7 @@
         <v>0.73755656108597278</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>6000</v>
       </c>
@@ -7555,7 +7829,7 @@
         <v>0.73636363636363633</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>6500</v>
       </c>
@@ -7570,7 +7844,7 @@
         <v>0.69777777777777783</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>7000</v>
       </c>
@@ -7585,7 +7859,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>7500</v>
       </c>
@@ -7600,7 +7874,7 @@
         <v>0.61027837259100648</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>8000</v>
       </c>
@@ -7615,7 +7889,7 @@
         <v>0.57234042553191489</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>8500</v>
       </c>
@@ -7630,7 +7904,7 @@
         <v>0.53829787234042548</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>9000</v>
       </c>
@@ -7645,7 +7919,7 @@
         <v>0.50736842105263158</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>9500</v>
       </c>
@@ -7660,7 +7934,7 @@
         <v>0.47708333333333336</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>10000</v>
       </c>
@@ -7675,7 +7949,7 @@
         <v>0.45154639175257733</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>500</v>
       </c>
@@ -7690,7 +7964,7 @@
         <v>7.0588235294117646E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>1000</v>
       </c>
@@ -7705,7 +7979,7 @@
         <v>0.14019607843137255</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>1500</v>
       </c>
@@ -7720,7 +7994,7 @@
         <v>0.21372549019607845</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>2000</v>
       </c>
@@ -7735,7 +8009,7 @@
         <v>0.28910891089108909</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>2500</v>
       </c>
@@ -7750,7 +8024,7 @@
         <v>0.37755102040816324</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>11000</v>
       </c>
@@ -7765,7 +8039,7 @@
         <v>0.4020408163265306</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>12000</v>
       </c>
@@ -7780,7 +8054,7 @@
         <v>0.36565656565656568</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>13000</v>
       </c>
@@ -7795,7 +8069,7 @@
         <v>0.32999999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>14000</v>
       </c>
@@ -7810,7 +8084,7 @@
         <v>0.30297029702970296</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>15000</v>
       </c>
@@ -7834,15 +8108,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -7852,8 +8126,11 @@
       <c r="C1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>5000</v>
       </c>
@@ -7863,8 +8140,14 @@
       <c r="C2">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E2">
+        <v>5340</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>5200</v>
       </c>
@@ -7874,8 +8157,14 @@
       <c r="C3">
         <v>1.1299999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E3">
+        <v>5340</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>5400</v>
       </c>
@@ -7886,7 +8175,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>5600</v>
       </c>
@@ -7897,7 +8186,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>5800</v>
       </c>
@@ -7908,7 +8197,7 @@
         <v>1.31</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>6000</v>
       </c>
@@ -7919,7 +8208,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>4500</v>
       </c>
@@ -7930,7 +8219,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>4000</v>
       </c>
@@ -7941,7 +8230,7 @@
         <v>2.5299999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>3500</v>
       </c>
@@ -7952,7 +8241,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>3000</v>
       </c>
@@ -7963,7 +8252,7 @@
         <v>3.76</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>6500</v>
       </c>
@@ -7974,7 +8263,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>7000</v>
       </c>
@@ -7985,7 +8274,7 @@
         <v>2.44</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>7500</v>
       </c>
@@ -7996,7 +8285,7 @@
         <v>2.81</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>8000</v>
       </c>

</xml_diff>